<commit_message>
PLAD Campaign & New smooshed smashed campaign
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateDeclines.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateDeclines.xlsx
@@ -1,27 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D5B6EF-FCE9-43CE-8CC3-18F0813AD6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="21075" windowHeight="8520"/>
+    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Reference number</t>
   </si>
@@ -63,12 +77,15 @@
   </si>
   <si>
     <t>Redeemed Date</t>
+  </si>
+  <si>
+    <t>Batch Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,7 +125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -136,44 +153,15 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -198,8 +186,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -218,9 +207,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,9 +247,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,7 +284,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,7 +319,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -503,152 +492,157 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="35.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.81640625" customWidth="1"/>
+    <col min="6" max="6" width="21.81640625" customWidth="1"/>
+    <col min="7" max="7" width="32.26953125" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" customWidth="1"/>
-    <col min="10" max="10" width="84.7109375" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="9" max="9" width="31.7265625" customWidth="1"/>
+    <col min="10" max="10" width="84.7265625" customWidth="1"/>
+    <col min="11" max="11" width="26.26953125" customWidth="1"/>
+    <col min="12" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:12" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="5.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="6"/>
+    <row r="2" spans="1:12" ht="5.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="6"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="7"/>
+    <row r="5" spans="1:12" ht="5.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="1"/>
+      <c r="C5" s="6"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="5.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="7"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="40" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup scale="39" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>